<commit_message>
isabelcalberti - Igualando nome das sheets
</commit_message>
<xml_diff>
--- a/ProcessoExcel/Resultados das vendas/ResultadosDasVendas-2024-01-15.xlsx
+++ b/ProcessoExcel/Resultados das vendas/ResultadosDasVendas-2024-01-15.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ifagundes\Documents\UiPath\ProcessoExcel\Resultados das vendas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ifagundes\Documents\UiPath-Study\ProcessoExcel\Resultados das vendas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E19CB68-5804-4AF9-B7BA-B3BA4376FC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7D0735-5AE3-4026-97EE-CEA12DAFC87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7D13614E-7C61-4E4D-8F2A-0760B32B995A}"/>
+    <workbookView xWindow="1896" yWindow="1980" windowWidth="11064" windowHeight="5700" activeTab="1" xr2:uid="{7D13614E-7C61-4E4D-8F2A-0760B32B995A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -446,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CFCA21-9A6E-4E83-98FB-C169DA7881FE}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:D81"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection sqref="A1:D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1595,4 +1596,16 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3CF918A-D2FE-47EB-A40B-9CD8CDAF2ABA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>